<commit_message>
force age to be numeric
</commit_message>
<xml_diff>
--- a/task_04/data_raw/candy_names_compare.xlsx
+++ b/task_04/data_raw/candy_names_compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\Malcolm\CodeClan\codeclan_project_malcolm_speight_dirty_data\task_04\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C063729E-DDBF-42C7-8890-1AC397AB9371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF282E9-7ED4-4F94-8F74-D268543162EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="14746" xr2:uid="{F222B2CF-0249-4841-B29D-77138B4BE405}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="127">
   <si>
     <t>Butterfinger</t>
   </si>
@@ -411,6 +411,9 @@
   </si>
   <si>
     <t>Exclude</t>
+  </si>
+  <si>
+    <t>New col name</t>
   </si>
 </sst>
 </file>
@@ -797,9 +800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936F4E1B-2D3A-41BD-979A-16C2A3601112}">
   <dimension ref="A1:I298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -833,6 +836,9 @@
       <c r="H1" s="6">
         <v>2017</v>
       </c>
+      <c r="I1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">

</xml_diff>